<commit_message>
Added LCC for hydraulic system in PluginLCA
</commit_message>
<xml_diff>
--- a/bim2sim/plugins/PluginHydraulicSystem/bim2sim_hydraulicsystem/assets/hydraulic_components.xlsx
+++ b/bim2sim/plugins/PluginHydraulicSystem/bim2sim_hydraulicsystem/assets/hydraulic_components.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\02_Git\bim2sim-Diss\bim2sim\bim2sim\plugins\PluginHydraulicSystem\bim2sim_hydraulicsystem\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dja-jho\Git\BIM2SIM\bim2sim\plugins\PluginHydraulicSystem\bim2sim_hydraulicsystem\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D648A74F-F6F9-410D-A398-5C406941DD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0AA8FD-BA87-4C97-99DB-5812BCE1B878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{AA4435EC-6D29-4471-A9A3-A3CE4E49EB19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AA4435EC-6D29-4471-A9A3-A3CE4E49EB19}"/>
   </bookViews>
   <sheets>
     <sheet name="Stahlrohre" sheetId="11" r:id="rId1"/>
     <sheet name="Kupferohre" sheetId="12" r:id="rId2"/>
-    <sheet name="Profilierte Flachheizkörper" sheetId="7" r:id="rId3"/>
+    <sheet name="Profilierte Flachheizkörper" sheetId="13" r:id="rId3"/>
     <sheet name="Fensterbankradiatoren" sheetId="2" r:id="rId4"/>
+    <sheet name="Profilierte Flachheizkörper alt" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,8 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="30">
   <si>
     <t>Normwärmeleistungen für Fensterbankradiatoren</t>
   </si>
@@ -121,6 +120,15 @@
   <si>
     <t>Außendurchmesser [mm]</t>
   </si>
+  <si>
+    <t>Trendlinie a</t>
+  </si>
+  <si>
+    <t>Trendlinie y = a * x ^ e</t>
+  </si>
+  <si>
+    <t>Trendlinie e</t>
+  </si>
 </sst>
 </file>
 
@@ -155,8 +163,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1804,26 +1816,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF4AC88-38D9-4C84-AD36-EA16909D4100}">
-  <dimension ref="A1:I22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB04C999-6321-48C7-9BF4-71DB06869876}">
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="11" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1851,497 +1856,414 @@
       <c r="I1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>65</v>
-      </c>
-      <c r="E2">
-        <v>1.25</v>
-      </c>
-      <c r="F2">
-        <v>436</v>
-      </c>
-      <c r="G2">
-        <v>2.7</v>
-      </c>
-      <c r="H2">
-        <v>11.6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>65</v>
-      </c>
-      <c r="E3">
-        <v>1.25</v>
-      </c>
-      <c r="F3">
-        <v>605</v>
-      </c>
-      <c r="G3">
-        <v>2.7</v>
-      </c>
-      <c r="H3">
-        <v>14.1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1.3</v>
+      </c>
+      <c r="F2" s="1">
+        <v>880</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="H2" s="1">
+        <v>21.3</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2">
+        <v>13120</v>
+      </c>
+      <c r="K2">
+        <v>-0.53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>350</v>
       </c>
-      <c r="B4">
+      <c r="B3" s="1">
         <v>300</v>
       </c>
-      <c r="C4">
+      <c r="C3" s="1">
+        <v>22</v>
+      </c>
+      <c r="D3" s="1">
+        <v>100</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1.3647</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1150</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2.8</v>
+      </c>
+      <c r="H3" s="1">
+        <v>25.2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3">
+        <v>15570</v>
+      </c>
+      <c r="K3">
+        <v>-0.54600000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
+        <v>33</v>
+      </c>
+      <c r="D4" s="1">
+        <v>155</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.3749</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1679</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H4" s="1">
+        <v>36.4</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4">
+        <v>16130</v>
+      </c>
+      <c r="K4">
+        <v>-0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
         <v>21</v>
       </c>
-      <c r="D4">
+      <c r="D5" s="1">
         <v>100</v>
       </c>
-      <c r="E4">
-        <v>1.27</v>
-      </c>
-      <c r="F4">
-        <v>915</v>
-      </c>
-      <c r="G4">
-        <v>5.4</v>
-      </c>
-      <c r="H4">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="I4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5">
+      <c r="E5" s="1">
+        <v>1.2867999999999999</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1082</v>
+      </c>
+      <c r="G5" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>26.3</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5">
+        <v>12711</v>
+      </c>
+      <c r="K5">
+        <v>-0.53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>500</v>
+      </c>
+      <c r="B6" s="1">
+        <v>450</v>
+      </c>
+      <c r="C6" s="1">
         <v>22</v>
       </c>
-      <c r="D5">
+      <c r="D6" s="1">
         <v>100</v>
       </c>
-      <c r="E5">
-        <v>1.28</v>
-      </c>
-      <c r="F5">
-        <v>1102</v>
-      </c>
-      <c r="G5">
-        <v>5.4</v>
-      </c>
-      <c r="H5">
-        <v>23.1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C6">
+      <c r="E6" s="1">
+        <v>1.3002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1380</v>
+      </c>
+      <c r="G6" s="1">
+        <v>3.6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>30.4</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6">
+        <v>13228</v>
+      </c>
+      <c r="K6">
+        <v>-0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
         <v>33</v>
       </c>
-      <c r="D6">
+      <c r="D7" s="1">
         <v>155</v>
       </c>
-      <c r="E6">
-        <v>1.3</v>
-      </c>
-      <c r="F6">
-        <v>1566</v>
-      </c>
-      <c r="G6">
-        <v>8.1</v>
-      </c>
-      <c r="H6">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="I6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7">
-        <v>65</v>
-      </c>
-      <c r="E7">
-        <v>1.25</v>
-      </c>
-      <c r="F7">
-        <v>586</v>
-      </c>
-      <c r="G7">
-        <v>3.5</v>
-      </c>
-      <c r="H7">
-        <v>15.2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C8">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>65</v>
-      </c>
-      <c r="E8">
-        <v>1.27</v>
-      </c>
-      <c r="F8">
-        <v>808</v>
-      </c>
-      <c r="G8">
-        <v>3.5</v>
-      </c>
-      <c r="H8">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>500</v>
-      </c>
-      <c r="B9">
-        <v>450</v>
-      </c>
-      <c r="C9">
+      <c r="E7" s="1">
+        <v>1.3167</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1978</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44.4</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7">
+        <v>15633</v>
+      </c>
+      <c r="K7">
+        <v>-0.51400000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1">
         <v>21</v>
       </c>
-      <c r="D9">
+      <c r="D8" s="1">
         <v>100</v>
       </c>
-      <c r="E9">
-        <v>1.3</v>
-      </c>
-      <c r="F9">
-        <v>1212</v>
-      </c>
-      <c r="G9">
-        <v>7</v>
-      </c>
-      <c r="H9">
-        <v>28.5</v>
-      </c>
-      <c r="I9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C10">
+      <c r="E8" s="1">
+        <v>1.3207</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1249</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H8" s="1">
+        <v>31.8</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8">
+        <v>11833</v>
+      </c>
+      <c r="K8">
+        <v>-0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>600</v>
+      </c>
+      <c r="B9" s="1">
+        <v>550</v>
+      </c>
+      <c r="C9" s="1">
         <v>22</v>
       </c>
-      <c r="D10">
+      <c r="D9" s="1">
         <v>100</v>
       </c>
-      <c r="E10">
-        <v>1.29</v>
-      </c>
-      <c r="F10">
-        <v>1461</v>
-      </c>
-      <c r="G10">
-        <v>7</v>
-      </c>
-      <c r="H10">
-        <v>32.700000000000003</v>
-      </c>
-      <c r="I10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C11">
+      <c r="E9" s="1">
+        <v>1.3162</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1629</v>
+      </c>
+      <c r="G9" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H9" s="1">
+        <v>36.1</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9">
+        <v>13943</v>
+      </c>
+      <c r="K9">
+        <v>-0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1">
         <v>33</v>
       </c>
-      <c r="D11">
+      <c r="D10" s="1">
         <v>155</v>
       </c>
-      <c r="E11">
-        <v>1.31</v>
-      </c>
-      <c r="F11">
-        <v>2124</v>
-      </c>
-      <c r="G11">
-        <v>10.5</v>
-      </c>
-      <c r="H11">
-        <v>48.7</v>
-      </c>
-      <c r="I11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>65</v>
-      </c>
-      <c r="E12">
-        <v>1.27</v>
-      </c>
-      <c r="F12">
-        <v>683</v>
-      </c>
-      <c r="G12">
-        <v>4</v>
-      </c>
-      <c r="H12">
-        <v>17.399999999999999</v>
-      </c>
-      <c r="I12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C13">
-        <v>11</v>
-      </c>
-      <c r="D13">
-        <v>65</v>
-      </c>
-      <c r="E13">
-        <v>1.28</v>
-      </c>
-      <c r="F13">
-        <v>943</v>
-      </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="H13">
-        <v>22.1</v>
-      </c>
-      <c r="I13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>600</v>
-      </c>
-      <c r="B14">
-        <v>550</v>
-      </c>
-      <c r="C14">
+      <c r="E10" s="1">
+        <v>1.3185</v>
+      </c>
+      <c r="F10" s="1">
+        <v>2233</v>
+      </c>
+      <c r="G10" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="H10" s="1">
+        <v>52.9</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10">
+        <v>13864</v>
+      </c>
+      <c r="K10">
+        <v>-0.497</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1">
         <v>21</v>
       </c>
-      <c r="D14">
+      <c r="D11" s="1">
         <v>100</v>
       </c>
-      <c r="E14">
-        <v>1.3</v>
-      </c>
-      <c r="F14">
-        <v>1406</v>
-      </c>
-      <c r="G14">
-        <v>8.1</v>
-      </c>
-      <c r="H14">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="I14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C15">
+      <c r="E11" s="1">
+        <v>1.3120000000000001</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1662</v>
+      </c>
+      <c r="G11" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="H11" s="1">
+        <v>45.1</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11">
+        <v>17882</v>
+      </c>
+      <c r="K11">
+        <v>-0.55900000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>900</v>
+      </c>
+      <c r="B12" s="1">
+        <v>850</v>
+      </c>
+      <c r="C12" s="1">
         <v>22</v>
       </c>
-      <c r="D15">
+      <c r="D12" s="1">
         <v>100</v>
       </c>
-      <c r="E15">
-        <v>1.3</v>
-      </c>
-      <c r="F15">
-        <v>1694</v>
-      </c>
-      <c r="G15">
-        <v>8.1</v>
-      </c>
-      <c r="H15">
-        <v>39</v>
-      </c>
-      <c r="I15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16">
+      <c r="E12" s="1">
+        <v>1.3185</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2109</v>
+      </c>
+      <c r="G12" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="H12" s="1">
+        <v>51.4</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12">
+        <v>13993</v>
+      </c>
+      <c r="K12">
+        <v>-0.502</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1">
         <v>33</v>
       </c>
-      <c r="D16">
+      <c r="D13" s="1">
         <v>155</v>
       </c>
-      <c r="E16">
-        <v>1.31</v>
-      </c>
-      <c r="F16">
-        <v>2461</v>
-      </c>
-      <c r="G16">
-        <v>12.1</v>
-      </c>
-      <c r="H16">
-        <v>58.1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>10</v>
-      </c>
-      <c r="D17">
-        <v>65</v>
-      </c>
-      <c r="E17">
-        <v>1.29</v>
-      </c>
-      <c r="F17">
-        <v>978</v>
-      </c>
-      <c r="G17">
-        <v>5.6</v>
-      </c>
-      <c r="H17">
-        <v>24.3</v>
-      </c>
-      <c r="I17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>11</v>
-      </c>
-      <c r="D18">
-        <v>65</v>
-      </c>
-      <c r="E18">
-        <v>1.3</v>
-      </c>
-      <c r="F18">
-        <v>1345</v>
-      </c>
-      <c r="G18">
-        <v>5.6</v>
-      </c>
-      <c r="H18">
-        <v>31.5</v>
-      </c>
-      <c r="I18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>900</v>
-      </c>
-      <c r="B19">
-        <v>850</v>
-      </c>
-      <c r="C19">
-        <v>21</v>
-      </c>
-      <c r="D19">
-        <v>100</v>
-      </c>
-      <c r="E19">
-        <v>1.3</v>
-      </c>
-      <c r="F19">
-        <v>1961</v>
-      </c>
-      <c r="G19">
-        <v>11.3</v>
-      </c>
-      <c r="H19">
-        <v>49.9</v>
-      </c>
-      <c r="I19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C20">
-        <v>22</v>
-      </c>
-      <c r="D20">
-        <v>100</v>
-      </c>
-      <c r="E20">
-        <v>1.32</v>
-      </c>
-      <c r="F20">
-        <v>2355</v>
-      </c>
-      <c r="G20">
-        <v>11.3</v>
-      </c>
-      <c r="H20">
-        <v>57.8</v>
-      </c>
-      <c r="I20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>33</v>
-      </c>
-      <c r="D21">
-        <v>155</v>
-      </c>
-      <c r="E21">
-        <v>1.32</v>
-      </c>
-      <c r="F21">
-        <v>3315</v>
-      </c>
-      <c r="G21">
-        <v>16.899999999999999</v>
-      </c>
-      <c r="H21">
-        <v>86.2</v>
-      </c>
-      <c r="I21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E13" s="1">
+        <v>1.3179000000000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2930</v>
+      </c>
+      <c r="G13" s="1">
+        <v>9.6</v>
+      </c>
+      <c r="H13" s="1">
+        <v>75</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13">
+        <v>15007</v>
+      </c>
+      <c r="K13">
+        <v>-0.46899999999999997</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2350,7 +2272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29E6B0A8-2D67-4CB1-A187-32AB4D6088EE}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
@@ -2998,4 +2920,547 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EF4AC88-38D9-4C84-AD36-EA16909D4100}">
+  <dimension ref="A1:I22"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>65</v>
+      </c>
+      <c r="E2">
+        <v>1.25</v>
+      </c>
+      <c r="F2">
+        <v>436</v>
+      </c>
+      <c r="G2">
+        <v>2.7</v>
+      </c>
+      <c r="H2">
+        <v>11.6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>65</v>
+      </c>
+      <c r="E3">
+        <v>1.25</v>
+      </c>
+      <c r="F3">
+        <v>605</v>
+      </c>
+      <c r="G3">
+        <v>2.7</v>
+      </c>
+      <c r="H3">
+        <v>14.1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>350</v>
+      </c>
+      <c r="B4">
+        <v>300</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>1.27</v>
+      </c>
+      <c r="F4">
+        <v>915</v>
+      </c>
+      <c r="G4">
+        <v>5.4</v>
+      </c>
+      <c r="H4">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>1.28</v>
+      </c>
+      <c r="F5">
+        <v>1102</v>
+      </c>
+      <c r="G5">
+        <v>5.4</v>
+      </c>
+      <c r="H5">
+        <v>23.1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>155</v>
+      </c>
+      <c r="E6">
+        <v>1.3</v>
+      </c>
+      <c r="F6">
+        <v>1566</v>
+      </c>
+      <c r="G6">
+        <v>8.1</v>
+      </c>
+      <c r="H6">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="I6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>65</v>
+      </c>
+      <c r="E7">
+        <v>1.25</v>
+      </c>
+      <c r="F7">
+        <v>586</v>
+      </c>
+      <c r="G7">
+        <v>3.5</v>
+      </c>
+      <c r="H7">
+        <v>15.2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>65</v>
+      </c>
+      <c r="E8">
+        <v>1.27</v>
+      </c>
+      <c r="F8">
+        <v>808</v>
+      </c>
+      <c r="G8">
+        <v>3.5</v>
+      </c>
+      <c r="H8">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>500</v>
+      </c>
+      <c r="B9">
+        <v>450</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>1.3</v>
+      </c>
+      <c r="F9">
+        <v>1212</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>28.5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>1.29</v>
+      </c>
+      <c r="F10">
+        <v>1461</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="I10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>155</v>
+      </c>
+      <c r="E11">
+        <v>1.31</v>
+      </c>
+      <c r="F11">
+        <v>2124</v>
+      </c>
+      <c r="G11">
+        <v>10.5</v>
+      </c>
+      <c r="H11">
+        <v>48.7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>65</v>
+      </c>
+      <c r="E12">
+        <v>1.27</v>
+      </c>
+      <c r="F12">
+        <v>683</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <v>65</v>
+      </c>
+      <c r="E13">
+        <v>1.28</v>
+      </c>
+      <c r="F13">
+        <v>943</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>22.1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>600</v>
+      </c>
+      <c r="B14">
+        <v>550</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14">
+        <v>1.3</v>
+      </c>
+      <c r="F14">
+        <v>1406</v>
+      </c>
+      <c r="G14">
+        <v>8.1</v>
+      </c>
+      <c r="H14">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="I14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
+      <c r="E15">
+        <v>1.3</v>
+      </c>
+      <c r="F15">
+        <v>1694</v>
+      </c>
+      <c r="G15">
+        <v>8.1</v>
+      </c>
+      <c r="H15">
+        <v>39</v>
+      </c>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>33</v>
+      </c>
+      <c r="D16">
+        <v>155</v>
+      </c>
+      <c r="E16">
+        <v>1.31</v>
+      </c>
+      <c r="F16">
+        <v>2461</v>
+      </c>
+      <c r="G16">
+        <v>12.1</v>
+      </c>
+      <c r="H16">
+        <v>58.1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>65</v>
+      </c>
+      <c r="E17">
+        <v>1.29</v>
+      </c>
+      <c r="F17">
+        <v>978</v>
+      </c>
+      <c r="G17">
+        <v>5.6</v>
+      </c>
+      <c r="H17">
+        <v>24.3</v>
+      </c>
+      <c r="I17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18">
+        <v>65</v>
+      </c>
+      <c r="E18">
+        <v>1.3</v>
+      </c>
+      <c r="F18">
+        <v>1345</v>
+      </c>
+      <c r="G18">
+        <v>5.6</v>
+      </c>
+      <c r="H18">
+        <v>31.5</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>900</v>
+      </c>
+      <c r="B19">
+        <v>850</v>
+      </c>
+      <c r="C19">
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <v>100</v>
+      </c>
+      <c r="E19">
+        <v>1.3</v>
+      </c>
+      <c r="F19">
+        <v>1961</v>
+      </c>
+      <c r="G19">
+        <v>11.3</v>
+      </c>
+      <c r="H19">
+        <v>49.9</v>
+      </c>
+      <c r="I19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20">
+        <v>1.32</v>
+      </c>
+      <c r="F20">
+        <v>2355</v>
+      </c>
+      <c r="G20">
+        <v>11.3</v>
+      </c>
+      <c r="H20">
+        <v>57.8</v>
+      </c>
+      <c r="I20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>33</v>
+      </c>
+      <c r="D21">
+        <v>155</v>
+      </c>
+      <c r="E21">
+        <v>1.32</v>
+      </c>
+      <c r="F21">
+        <v>3315</v>
+      </c>
+      <c r="G21">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="H21">
+        <v>86.2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>